<commit_message>
BIS-768: Fixed XLS export test files
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Multivalued</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique</t>
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
@@ -207,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -224,7 +227,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -240,124 +251,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4:L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -417,92 +322,104 @@
       <c r="K4" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="L4" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="4" t="s">
-        <v>16</v>
+      <c r="K5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="4" t="s">
-        <v>16</v>
+      <c r="K6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="4" t="s">
-        <v>16</v>
+      <c r="K7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BIS-769: Fixed xls test files
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">Unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern Type</t>
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
@@ -256,13 +262,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4:L7"/>
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4:N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -325,101 +331,107 @@
       <c r="L4" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="M4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BIS-1002: Fixed XLS export tests
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pattern Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Assignment</t>
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
@@ -129,7 +132,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -168,6 +171,14 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -216,7 +227,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +245,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -262,13 +277,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4:N4"/>
+      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -337,101 +352,113 @@
       <c r="N4" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="O4" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>19</v>
+      <c r="K5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>19</v>
+      <c r="K6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>19</v>
+      <c r="K7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BIS-1002: removed "Internal Assignment" column from export. Expanded and fixed tests
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pattern Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internal Assignment</t>
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
@@ -283,7 +280,7 @@
       <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -352,114 +349,106 @@
       <c r="N4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="O7" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
BIS-1630: Fixed xls export tests
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Internal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
@@ -37,6 +40,9 @@
     <t xml:space="preserve">ATTACHMENT</t>
   </si>
   <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attachment</t>
   </si>
   <si>
@@ -76,10 +82,10 @@
     <t xml:space="preserve">Pattern Type</t>
   </si>
   <si>
-    <t xml:space="preserve">$NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
+    <t xml:space="preserve">Internal Assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME</t>
   </si>
   <si>
     <t xml:space="preserve">TRUE</t>
@@ -109,7 +115,7 @@
     <t xml:space="preserve">{"custom_widget":"Word Processor"}</t>
   </si>
   <si>
-    <t xml:space="preserve">$XMLCOMMENTS</t>
+    <t xml:space="preserve">XMLCOMMENTS</t>
   </si>
   <si>
     <t xml:space="preserve">Comments List</t>
@@ -129,7 +135,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -160,9 +166,22 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -224,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,11 +260,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,181 +301,207 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4:O7"/>
+      <selection pane="topLeft" activeCell="P4" activeCellId="0" sqref="P4:P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="L4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="M4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="5"/>
+      <c r="N4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="2"/>
+      <c r="G6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" s="2"/>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>